<commit_message>
All paths of a tree - Iterative approach, Genius
</commit_message>
<xml_diff>
--- a/IDEAS generated from LeetCode.xlsx
+++ b/IDEAS generated from LeetCode.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My tutorials\python coursera\practice\Leetcode and Hackerrank\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C7E7ED6-E7B4-400B-AF1C-E0FA07EF4E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0CA2D8-AB53-4DAE-BD4C-B6AF719E76D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Two Sum</t>
   </si>
@@ -62,13 +61,20 @@
   <si>
     <t>Object oriented -New paramater should be defined in the __init__ with self
 Other functions must get para with self.blah blah</t>
+  </si>
+  <si>
+    <t>57. Insert Interval</t>
+  </si>
+  <si>
+    <t>start from non overlapping, ie, the head of the newInterval first, then the its tail ,finally work
+on the overlapping one (75 questions folder contains the answer)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,8 +121,14 @@
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF262626"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -147,6 +159,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -160,7 +178,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -200,6 +218,12 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -483,8 +507,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:F103"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -561,9 +585,16 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:6" ht="83.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="3">
         <v>7</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="15"/>
+      <c r="F10" s="8" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
level order traversal in Trees - 2D array output
</commit_message>
<xml_diff>
--- a/IDEAS generated from LeetCode.xlsx
+++ b/IDEAS generated from LeetCode.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My tutorials\python coursera\practice\Leetcode and Hackerrank\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D0CA2D8-AB53-4DAE-BD4C-B6AF719E76D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC30BCC-8474-4281-84B8-D7B696311B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Two Sum</t>
   </si>
@@ -68,6 +68,12 @@
   <si>
     <t>start from non overlapping, ie, the head of the newInterval first, then the its tail ,finally work
 on the overlapping one (75 questions folder contains the answer)</t>
+  </si>
+  <si>
+    <t>102 level order traversal</t>
+  </si>
+  <si>
+    <t>create 2D elems for the stack,2nd member representing the level ~  stack=[ [node,0] ]</t>
   </si>
 </sst>
 </file>
@@ -508,7 +514,7 @@
   <dimension ref="B4:F103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -601,6 +607,13 @@
       <c r="B11" s="4">
         <v>8</v>
       </c>
+      <c r="C11" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="6"/>
+      <c r="F11" s="7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B12" s="4">

</xml_diff>

<commit_message>
some trees and arrays
</commit_message>
<xml_diff>
--- a/IDEAS generated from LeetCode.xlsx
+++ b/IDEAS generated from LeetCode.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My tutorials\python coursera\practice\Leetcode and Hackerrank\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC30BCC-8474-4281-84B8-D7B696311B0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E29C104-7961-4398-B0BB-0B0F84E11B05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Two Sum</t>
   </si>
@@ -74,6 +74,13 @@
   </si>
   <si>
     <t>create 2D elems for the stack,2nd member representing the level ~  stack=[ [node,0] ]</t>
+  </si>
+  <si>
+    <t>15. 3Sum</t>
+  </si>
+  <si>
+    <t>create and obj, keys will be value of the nums, values will be 2D arrays representing
+i and -nums[k]-nums[i]. Some sortings are required for non-repetitives</t>
   </si>
 </sst>
 </file>
@@ -513,8 +520,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B4:F103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
@@ -615,9 +622,16 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:6" ht="36" x14ac:dyDescent="0.3">
       <c r="B12" s="4">
         <v>9</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="15"/>
+      <c r="F12" s="8" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.3">

</xml_diff>